<commit_message>
Subiendo archivo desde Python
</commit_message>
<xml_diff>
--- a/nucleo/nucleo.xlsx
+++ b/nucleo/nucleo.xlsx
@@ -20,7 +20,7 @@
     <t>Exportado:</t>
   </si>
   <si>
-    <t>sáb. 03/05/2025 19:26</t>
+    <t>mié. 07/05/2025 19:09</t>
   </si>
   <si>
     <t>Fecha</t>
@@ -104,8 +104,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Datos" displayName="Datos" ref="A5:D38" headerRowCount="1" totalsRowCount="1">
-  <autoFilter ref="A5:D37"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Datos" displayName="Datos" ref="A5:D42" headerRowCount="1" totalsRowCount="1">
+  <autoFilter ref="A5:D41"/>
   <tableColumns count="4">
     <tableColumn id="1" name="Fecha"/>
     <tableColumn id="2" name="Cantidad de pedidos" totalsRowFunction="sum"/>
@@ -118,7 +118,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:D38"/>
+  <dimension ref="A1:D42"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -620,14 +620,70 @@
       </c>
     </row>
     <row r="38">
-      <c r="A38" s="7"/>
-      <c r="B38" s="4">
+      <c r="A38" s="5">
+        <v>45780</v>
+      </c>
+      <c r="B38" s="0">
+        <v>19</v>
+      </c>
+      <c r="C38" s="0">
+        <v>418500</v>
+      </c>
+      <c r="D38" s="0">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" s="5">
+        <v>45781</v>
+      </c>
+      <c r="B39" s="0">
+        <v>12</v>
+      </c>
+      <c r="C39" s="0">
+        <v>201200</v>
+      </c>
+      <c r="D39" s="0">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" s="5">
+        <v>45783</v>
+      </c>
+      <c r="B40" s="0">
+        <v>14</v>
+      </c>
+      <c r="C40" s="0">
+        <v>275800</v>
+      </c>
+      <c r="D40" s="0">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" s="5">
+        <v>45784</v>
+      </c>
+      <c r="B41" s="0">
+        <v>3</v>
+      </c>
+      <c r="C41" s="0">
+        <v>55500</v>
+      </c>
+      <c r="D41" s="0">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" s="7"/>
+      <c r="B42" s="4">
         <f>SUBTOTAL(109,Datos[Cantidad de pedidos])</f>
       </c>
-      <c r="C38" s="4">
+      <c r="C42" s="4">
         <f>SUBTOTAL(109,Datos[Total $])</f>
       </c>
-      <c r="D38" s="4">
+      <c r="D42" s="4">
         <f>SUBTOTAL(109,Datos[Cantidad de productos])</f>
       </c>
     </row>

</xml_diff>